<commit_message>
Python comprehensions and Random variables
</commit_message>
<xml_diff>
--- a/التأليف والتفكيك.xlsx
+++ b/التأليف والتفكيك.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20106\PycharmProjects\Data-Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32090FC-9939-4D4A-B0BA-A3DD53E4B6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F179AD-06FD-4B7B-90E7-0FE3218ABE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="هندسة البيانات" sheetId="4" r:id="rId1"/>
     <sheet name="علم البيانات" sheetId="5" r:id="rId2"/>
+    <sheet name="رياضيات" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>connect</t>
   </si>
@@ -82,6 +83,12 @@
   </si>
   <si>
     <t>نموذج انحدار خطي ++ =&gt; أي أضيف للمدخلات بتاعته أس</t>
+  </si>
+  <si>
+    <t>Random Variables المتغيرات العشوائية</t>
+  </si>
+  <si>
+    <t>ما يكافئ الدالة لكن في الاحتمالات؛ حيث أن الدالة نتيجتها حتمية؛ بينما المتغير العشوائي نتيجته غير حتمية ولا متوقعة وعشوائية</t>
   </si>
 </sst>
 </file>
@@ -28401,7 +28408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0012A1-0841-43F8-AC82-7A12528A682E}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -28422,4 +28429,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83229F82-1901-407C-BF29-A7A9E3BD1211}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="89.77734375" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bayes' rule vs joint probability distribution
</commit_message>
<xml_diff>
--- a/التأليف والتفكيك.xlsx
+++ b/التأليف والتفكيك.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20106\PycharmProjects\Data-Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B644A9-803F-42A0-8F85-BB237C7D664C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAEAEDF-4C2E-434A-ABDF-8F48C08C3F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>connect</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>مش قاعدة؛ الكلام ده ممكن يكون صح عند الغير مهندسين اللي بيبيقى عندهم مشكلة في هذا الأمر</t>
+  </si>
+  <si>
+    <t>Probability Distribution</t>
+  </si>
+  <si>
+    <t>Enterprise</t>
+  </si>
+  <si>
+    <t>تجد نقطة ال agility حاضرة فيها كما كانت حاضرة في rework: the world is constantly changing, and predicting the future is impossible</t>
   </si>
 </sst>
 </file>
@@ -366,13 +375,13 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="3"/>
+    <col min="1" max="1" width="20" style="3" customWidth="1"/>
     <col min="2" max="2" width="167.5546875" style="3" customWidth="1"/>
     <col min="3" max="16384" width="12.6640625" style="3"/>
   </cols>
@@ -537,7 +546,7 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -601,7 +610,7 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -634,8 +643,12 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -28419,7 +28432,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -28443,10 +28456,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83229F82-1901-407C-BF29-A7A9E3BD1211}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -28464,6 +28477,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="2" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Scrapping football t-shirts websites
</commit_message>
<xml_diff>
--- a/التأليف والتفكيك.xlsx
+++ b/التأليف والتفكيك.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20106\PycharmProjects\Data-Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAEAEDF-4C2E-434A-ABDF-8F48C08C3F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7C8D24-092B-4E1C-AF53-D31537A83680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>connect</t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t>تجد نقطة ال agility حاضرة فيها كما كانت حاضرة في rework: the world is constantly changing, and predicting the future is impossible</t>
+  </si>
+  <si>
+    <t>Bayes' rule vs joint distribution distribution</t>
+  </si>
+  <si>
+    <t>نستغني عن ال bayes' rule لما يكون معنا ال joint probability distribution</t>
+  </si>
+  <si>
+    <t>Golden rule</t>
+  </si>
+  <si>
+    <t>Technical solutions exist not for their own sake but in support of business goals.</t>
   </si>
 </sst>
 </file>
@@ -375,8 +387,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -675,8 +687,12 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -28456,10 +28472,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83229F82-1901-407C-BF29-A7A9E3BD1211}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -28482,6 +28498,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="3" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Likelihood function not likelihood distribution
</commit_message>
<xml_diff>
--- a/التأليف والتفكيك.xlsx
+++ b/التأليف والتفكيك.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20106\PycharmProjects\Data-Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7C8D24-092B-4E1C-AF53-D31537A83680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684A0F90-5F74-4D67-88D9-BBA7760FB3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11412" yWindow="0" windowWidth="11724" windowHeight="12336" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="هندسة البيانات" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>connect</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>Technical solutions exist not for their own sake but in support of business goals.</t>
+  </si>
+  <si>
+    <t>Likelihood function or likelihood distribution?</t>
+  </si>
+  <si>
+    <t>a function and a distribution because probability distributions must add up to one (or integrate to one if we are dealing with continuous random variables), but the likelihood function does not necessarily add up to one (or integrate to one in the case of continuous random variables)</t>
   </si>
 </sst>
 </file>
@@ -387,7 +393,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -28472,10 +28478,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83229F82-1901-407C-BF29-A7A9E3BD1211}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -28506,6 +28512,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="4" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Terminology in Data Engineering, what is a pipeline, Airflow and NiFi.
</commit_message>
<xml_diff>
--- a/التأليف والتفكيك.xlsx
+++ b/التأليف والتفكيك.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20106\PycharmProjects\Data-Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0406219-E245-4BCA-A6EE-6388684BF860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D049FFB-B739-4D3F-849E-A86192B2C789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="هندسة البيانات" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>connect</t>
   </si>
@@ -129,6 +129,30 @@
   </si>
   <si>
     <t>cloud-based AI services (AWS, GCP, Azure)</t>
+  </si>
+  <si>
+    <t>Data Pipeline</t>
+  </si>
+  <si>
+    <t>تجميعة الداتا بيز مع لغة برمحة مع warehouse مع processing engine + حاجه تخلي كل العملية تمشي تلقائي (scheduler)</t>
+  </si>
+  <si>
+    <t>Crontab</t>
+  </si>
+  <si>
+    <t>منظم عملية الشغل التلقائي لل pipeline باستخدام ما يسمى cron jobs… اعتبره زي دوكر؛ مينفعش تعتمد عليه لواحده؛ يعملك وجع دماغك =&gt; محتاج orchisteration</t>
+  </si>
+  <si>
+    <t>Apache Airflow</t>
+  </si>
+  <si>
+    <t>Apache NiFi</t>
+  </si>
+  <si>
+    <t>web server, a scheduler, a metastore, a queueing system, and executors. |&gt; Batch/ML pipelines</t>
+  </si>
+  <si>
+    <t>Dataflow tool هيستخدمها في الكتاب بدلا من الأيرفلو    |&gt; ETL/Streaming | طريقة أخرى لبناء ال pipelines</t>
   </si>
 </sst>
 </file>
@@ -400,8 +424,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -732,8 +756,12 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -760,8 +788,12 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -788,8 +820,12 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -816,8 +852,12 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -28536,7 +28576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230B57E5-7C82-4839-942B-B4D596D3F486}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Difference between 0 cor,cov and independence
</commit_message>
<xml_diff>
--- a/التأليف والتفكيك.xlsx
+++ b/التأليف والتفكيك.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20106\PycharmProjects\Data-Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D049FFB-B739-4D3F-849E-A86192B2C789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5BD087-3BBA-46A6-9DD1-5A9E5DDC5B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="هندسة البيانات" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>connect</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>Dataflow tool هيستخدمها في الكتاب بدلا من الأيرفلو    |&gt; ETL/Streaming | طريقة أخرى لبناء ال pipelines</t>
+  </si>
+  <si>
+    <t>Zero correlation|covariance XX Independence</t>
+  </si>
+  <si>
+    <t>0 cor|cov = linear independence |But| independence is stronger</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -28525,10 +28531,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83229F82-1901-407C-BF29-A7A9E3BD1211}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -28565,6 +28571,14 @@
       </c>
       <c r="B4" s="3" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>